<commit_message>
Keep to 1 u joint steering, lookup table steering gives a few issues and does not turn properly
</commit_message>
<xml_diff>
--- a/Scripts_Data/Data_Vehicle/ARTTU.xlsx
+++ b/Scripts_Data/Data_Vehicle/ARTTU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Desktop/FSAE/Motor Control/VehicleModel/Scripts_Data/Data_Vehicle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Desktop/FSAE/Vehicle Model/Main/Develop/Scripts_Data/Data_Vehicle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF3101-8249-CE4D-866D-452CCC23842D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA83AF4-EF73-7D47-88BD-934E260F22E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="1360" windowWidth="25360" windowHeight="18980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="1360" windowWidth="25360" windowHeight="18980" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -5112,8 +5112,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="109" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView showGridLines="0" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5178,7 +5178,7 @@
         <v>588.50099999999998</v>
       </c>
       <c r="D4" s="97">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="76"/>
     </row>
@@ -5483,8 +5483,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5654,7 +5654,7 @@
         <v>578</v>
       </c>
       <c r="D11" s="97">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E11" s="76"/>
     </row>

</xml_diff>